<commit_message>
Added a "implemented" column
</commit_message>
<xml_diff>
--- a/assets/sounds/soundMasterList.xlsx
+++ b/assets/sounds/soundMasterList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Trigger</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>wooshing sound</t>
+  </si>
+  <si>
+    <t>Implemented?</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,9 +450,10 @@
     <col min="2" max="2" width="48.77734375" customWidth="1"/>
     <col min="3" max="3" width="39.21875" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -460,10 +464,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -474,8 +481,9 @@
         <v>17</v>
       </c>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -486,8 +494,9 @@
         <v>18</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -498,8 +507,9 @@
         <v>16</v>
       </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -510,8 +520,9 @@
         <v>19</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -522,8 +533,9 @@
         <v>20</v>
       </c>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -534,6 +546,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>